<commit_message>
new code and new analysis 2013_12_24_1:29
</commit_message>
<xml_diff>
--- a/log/动静一级OMP_CUDA_动态参数_实验测试表.xlsx
+++ b/log/动静一级OMP_CUDA_动态参数_实验测试表.xlsx
@@ -16,53 +16,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>华硕K40IN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>chuan50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chuan100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chuan600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chuan4000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位：秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_动_无动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_静_无动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_动静_无动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_动_有动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_静_有动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPS_动静_有动参</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>动_无动参</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>静_无动参</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>动_有动参</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>动静_有动参</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chuan50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chuan100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chuan600</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chuan4000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>动静_无动参</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>静_有动参</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单位：秒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -409,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -425,26 +433,26 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>13.946</v>
@@ -461,7 +469,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>13.680999999999999</v>
@@ -478,7 +486,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>14.554</v>
@@ -495,7 +503,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -505,7 +513,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>